<commit_message>
add data filtering code
</commit_message>
<xml_diff>
--- a/check/redcap_checks.xlsx
+++ b/check/redcap_checks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominick\Documents\UFHealth_EHR\check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinsongdu/mnt/projects/UFHealth/check/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65A53C0-DF6E-224D-957A-40C25744D2F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="860" yWindow="2800" windowWidth="26200" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>instrument</t>
   </si>
@@ -207,19 +208,72 @@
   </si>
   <si>
     <t>27800 E669 Z6854 E6601 V8554 Z6853 27801 V8553</t>
+  </si>
+  <si>
+    <t>465.8',
+ '465.9',
+ '466',
+ '491.21',
+ '493',
+ '493.01',
+ '493.02',
+ '493.1',
+ '493.11',
+ '493.2',
+ '493.81',
+ '493.82',
+ '493.9',
+ '493.91',
+ '493.92',
+ 'J06.9',
+ 'J20.9',
+ 'J44.1',
+ 'J44.9',
+ 'J45.20',
+ 'J45.21',
+ 'J45.22',
+ 'J45.30',
+ 'J45.31',
+ 'J45.32',
+ 'J45.40',
+ 'J45.41',
+ 'J45.42',
+ 'J45.50',
+ 'J45.51',
+ 'J45.52',
+ 'J45.901',
+ 'J45.902',
+ 'J45.909',
+ 'J45.991',
+ 'J45.998'</t>
+  </si>
+  <si>
+    <t>import_unique_icd</t>
+  </si>
+  <si>
+    <t>check_unique_icd</t>
+  </si>
+  <si>
+    <t>'466', '493', '493.1', '493.2', '493.9'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -242,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -250,6 +304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,30 +621,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +678,14 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -641,7 +705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -661,7 +725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -681,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -701,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -721,7 +785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -741,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -761,7 +825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -781,7 +845,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -801,7 +865,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -821,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -841,7 +905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -861,7 +925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -881,7 +945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -901,7 +965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -920,8 +984,26 @@
       <c r="F16" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>13241</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1">
+        <v>3577</v>
+      </c>
+      <c r="J16" s="1">
+        <v>75</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -941,7 +1023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -961,7 +1043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -981,7 +1063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1001,7 +1083,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1021,7 +1103,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1041,7 +1123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1061,7 +1143,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1081,7 +1163,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1101,7 +1183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1121,7 +1203,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1141,7 +1223,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1161,7 +1243,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1181,7 +1263,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1201,7 +1283,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1221,7 +1303,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1241,7 +1323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
initialize code for check and subsetting
</commit_message>
<xml_diff>
--- a/check/redcap_checks.xlsx
+++ b/check/redcap_checks.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinsongdu/mnt/projects/UFHealth/check/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65A53C0-DF6E-224D-957A-40C25744D2F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3D6E57-D698-5F4F-8A1F-FD4460174197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="2800" windowWidth="26200" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="2800" windowWidth="27660" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>instrument</t>
   </si>
@@ -256,12 +256,24 @@
   <si>
     <t>'466', '493', '493.1', '493.2', '493.9'</t>
   </si>
+  <si>
+    <t>30567 (16684 are baby ids with non-missing demographic information)</t>
+  </si>
+  <si>
+    <t>466.0', '493.00', '493.10', '493.20', '493.90'</t>
+  </si>
+  <si>
+    <t>16607 (RedCap Form: linked_mom_demography?)</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +286,11 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
   <fills count="2">
@@ -296,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -308,6 +325,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,11 +647,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -636,15 +659,17 @@
     <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="1"/>
+    <col min="12" max="12" width="24.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="32.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,7 +710,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -704,8 +729,20 @@
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="1">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -724,8 +761,20 @@
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>105611</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>13068</v>
+      </c>
+      <c r="J3" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -744,8 +793,20 @@
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G4" s="1">
+        <v>51441</v>
+      </c>
+      <c r="H4" s="1">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7667</v>
+      </c>
+      <c r="J4" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -764,8 +825,14 @@
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -784,8 +851,20 @@
       <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G6" s="1">
+        <v>16441</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6</v>
+      </c>
+      <c r="I6" s="1">
+        <v>16441</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -804,8 +883,20 @@
       <c r="F7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G7" s="1">
+        <v>16353</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>16346</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -824,8 +915,20 @@
       <c r="F8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G8" s="1">
+        <v>5156</v>
+      </c>
+      <c r="H8" s="1">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2721</v>
+      </c>
+      <c r="J8" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -844,8 +947,20 @@
       <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G9" s="1">
+        <v>70367</v>
+      </c>
+      <c r="H9" s="1">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1">
+        <v>15998</v>
+      </c>
+      <c r="J9" s="1">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -864,8 +979,20 @@
       <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="G10" s="1">
+        <v>51398</v>
+      </c>
+      <c r="H10" s="1">
+        <v>6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>6740</v>
+      </c>
+      <c r="J10" s="1">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -885,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="16">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -905,7 +1032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="16">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -925,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="16">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -945,7 +1072,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="16">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -965,7 +1092,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="120.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -999,11 +1126,14 @@
       <c r="K16" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="L16" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="M16" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="64">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="64">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="32.25" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1193,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1083,7 +1213,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -1103,7 +1233,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="28.5" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1253,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="30" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1143,7 +1273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="42.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1163,7 +1293,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="112">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1182,8 +1312,23 @@
       <c r="F25" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G25" s="1">
+        <v>5293</v>
+      </c>
+      <c r="H25" s="1">
+        <v>6</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2465</v>
+      </c>
+      <c r="J25" s="1">
+        <v>29</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="32">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1203,7 +1348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="48">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1223,7 +1368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="48">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1243,7 +1388,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="48">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1263,7 +1408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="32">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1428,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="32">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1303,7 +1448,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="32">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1323,7 +1468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="16">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>